<commit_message>
Add an E-stop monitor (MC4) and CP command posibility (MC5).
</commit_message>
<xml_diff>
--- a/Documentation/PLC variables.xlsx
+++ b/Documentation/PLC variables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="178">
   <si>
     <t>Device</t>
   </si>
@@ -51,15 +51,15 @@
     <t>show key position</t>
   </si>
   <si>
+    <t>C2</t>
+  </si>
+  <si>
     <t>Door status</t>
   </si>
   <si>
     <t>Door open/close</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>Door power</t>
   </si>
   <si>
@@ -78,336 +78,342 @@
     <t>C4</t>
   </si>
   <si>
+    <t>E-stop ind</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>E-stop modbus</t>
+  </si>
+  <si>
+    <t>Lights</t>
+  </si>
+  <si>
+    <t>C235</t>
+  </si>
+  <si>
+    <t>Control room lights new status</t>
+  </si>
+  <si>
+    <t>Changes relay</t>
+  </si>
+  <si>
+    <t>C236</t>
+  </si>
+  <si>
+    <t>Utilities room lights new status</t>
+  </si>
+  <si>
+    <t>C237</t>
+  </si>
+  <si>
+    <t>Spectrograph room lights new status</t>
+  </si>
+  <si>
+    <t>C238</t>
+  </si>
+  <si>
+    <t>UMA lights new status</t>
+  </si>
+  <si>
+    <t>C239</t>
+  </si>
+  <si>
+    <t>Tel Plat bright lights new status</t>
+  </si>
+  <si>
+    <t>C240</t>
+  </si>
+  <si>
+    <t>Tel plat red new status</t>
+  </si>
+  <si>
+    <t>C335</t>
+  </si>
+  <si>
+    <t>Control room lights status</t>
+  </si>
+  <si>
+    <t>C336</t>
+  </si>
+  <si>
+    <t>Utilities room lights status</t>
+  </si>
+  <si>
+    <t>C337</t>
+  </si>
+  <si>
+    <t>Spectrograph room lights status</t>
+  </si>
+  <si>
+    <t>C338</t>
+  </si>
+  <si>
+    <t>UMA lights status</t>
+  </si>
+  <si>
+    <t>C339</t>
+  </si>
+  <si>
+    <t>Tel Plat bright lights status</t>
+  </si>
+  <si>
+    <t>C340</t>
+  </si>
+  <si>
+    <t>Tel plat red status</t>
+  </si>
+  <si>
+    <t>Shutter movement</t>
+  </si>
+  <si>
+    <t>C100</t>
+  </si>
+  <si>
+    <t>Drive enable</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>Drive state</t>
+  </si>
+  <si>
+    <t>C102</t>
+  </si>
+  <si>
+    <t>Motor direction</t>
+  </si>
+  <si>
+    <t>C103</t>
+  </si>
+  <si>
+    <t>Drive brake</t>
+  </si>
+  <si>
+    <t>D104-105</t>
+  </si>
+  <si>
+    <t>Drive velocity</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>NE limit switch status</t>
+  </si>
+  <si>
+    <t>C106</t>
+  </si>
+  <si>
+    <t>NW limit switch status</t>
+  </si>
+  <si>
+    <t>C107</t>
+  </si>
+  <si>
+    <t>SE limit switch status</t>
+  </si>
+  <si>
+    <t>C108</t>
+  </si>
+  <si>
+    <t>SW limit switch status</t>
+  </si>
+  <si>
+    <t>C110</t>
+  </si>
+  <si>
+    <t>Overcurrent</t>
+  </si>
+  <si>
+    <t>D120</t>
+  </si>
+  <si>
+    <t>Open timeout</t>
+  </si>
+  <si>
+    <t>D121</t>
+  </si>
+  <si>
+    <t>Close timeout</t>
+  </si>
+  <si>
+    <t>C122</t>
+  </si>
+  <si>
+    <t>Open small move timeout</t>
+  </si>
+  <si>
+    <t>C123</t>
+  </si>
+  <si>
+    <t>Close small move timeout</t>
+  </si>
+  <si>
+    <t>D130</t>
+  </si>
+  <si>
+    <t>Drive current</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>Timout_error</t>
+  </si>
+  <si>
+    <t>dxxx</t>
+  </si>
+  <si>
+    <t>dome Counter</t>
+  </si>
+  <si>
+    <t>domve velocity</t>
+  </si>
+  <si>
+    <t>Emergency stop</t>
+  </si>
+  <si>
+    <t>C200</t>
+  </si>
+  <si>
+    <t>E-Stop</t>
+  </si>
+  <si>
+    <t>C201</t>
+  </si>
+  <si>
+    <t>E-Stop status</t>
+  </si>
+  <si>
+    <t>C202</t>
+  </si>
+  <si>
+    <t>E-relay reset.</t>
+  </si>
+  <si>
+    <t>HVAC</t>
+  </si>
+  <si>
+    <t>D500</t>
+  </si>
+  <si>
+    <t>D101</t>
+  </si>
+  <si>
+    <t>X0</t>
+  </si>
+  <si>
+    <t>Safety key</t>
+  </si>
+  <si>
+    <t>Engaged?</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Open/Close</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Door Power</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>Shows actual driving state</t>
+  </si>
+  <si>
+    <t>X10</t>
+  </si>
+  <si>
+    <t>Control room lights curr det</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>Utilities room lights curr det</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>Spectrograph room lights curr det</t>
+  </si>
+  <si>
+    <t>X13</t>
+  </si>
+  <si>
+    <t>UMA lights curr det</t>
+  </si>
+  <si>
+    <t>X14</t>
+  </si>
+  <si>
+    <t>Tel Plat bright lights curr det</t>
+  </si>
+  <si>
+    <t>X15</t>
+  </si>
+  <si>
+    <t>Tel plat red curr det</t>
+  </si>
+  <si>
+    <t>X9</t>
+  </si>
+  <si>
+    <t>NE limit switch</t>
+  </si>
+  <si>
+    <t>NW limit switch</t>
+  </si>
+  <si>
+    <t>SE limit switch</t>
+  </si>
+  <si>
+    <t>SW limit switch</t>
+  </si>
+  <si>
+    <t>WX0</t>
+  </si>
+  <si>
+    <t>Motor counter</t>
+  </si>
+  <si>
+    <t>Y0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator light </t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Door magnet</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
     <t>E-stop</t>
   </si>
   <si>
-    <t>Lights</t>
-  </si>
-  <si>
-    <t>C235</t>
-  </si>
-  <si>
-    <t>Control room lights new status</t>
-  </si>
-  <si>
-    <t>Changes relay</t>
-  </si>
-  <si>
-    <t>C236</t>
-  </si>
-  <si>
-    <t>Utilities room lights new status</t>
-  </si>
-  <si>
-    <t>C237</t>
-  </si>
-  <si>
-    <t>Spectrograph room lights new status</t>
-  </si>
-  <si>
-    <t>C238</t>
-  </si>
-  <si>
-    <t>UMA lights new status</t>
-  </si>
-  <si>
-    <t>C239</t>
-  </si>
-  <si>
-    <t>Tel Plat bright lights new status</t>
-  </si>
-  <si>
-    <t>C240</t>
-  </si>
-  <si>
-    <t>Tel plat red new status</t>
-  </si>
-  <si>
-    <t>C335</t>
-  </si>
-  <si>
-    <t>Control room lights status</t>
-  </si>
-  <si>
-    <t>C336</t>
-  </si>
-  <si>
-    <t>Utilities room lights status</t>
-  </si>
-  <si>
-    <t>C337</t>
-  </si>
-  <si>
-    <t>Spectrograph room lights status</t>
-  </si>
-  <si>
-    <t>C338</t>
-  </si>
-  <si>
-    <t>UMA lights status</t>
-  </si>
-  <si>
-    <t>C339</t>
-  </si>
-  <si>
-    <t>Tel Plat bright lights status</t>
-  </si>
-  <si>
-    <t>C340</t>
-  </si>
-  <si>
-    <t>Tel plat red status</t>
-  </si>
-  <si>
-    <t>Shutter movement</t>
-  </si>
-  <si>
-    <t>C100</t>
-  </si>
-  <si>
-    <t>Drive enable</t>
-  </si>
-  <si>
-    <t>C101</t>
-  </si>
-  <si>
-    <t>Drive state</t>
-  </si>
-  <si>
-    <t>C102</t>
-  </si>
-  <si>
-    <t>Motor direction</t>
-  </si>
-  <si>
-    <t>C103</t>
-  </si>
-  <si>
-    <t>Drive brake</t>
-  </si>
-  <si>
-    <t>D104-105</t>
-  </si>
-  <si>
-    <t>Drive velocity</t>
-  </si>
-  <si>
-    <t>C105</t>
-  </si>
-  <si>
-    <t>NE limit switch status</t>
-  </si>
-  <si>
-    <t>C106</t>
-  </si>
-  <si>
-    <t>NW limit switch status</t>
-  </si>
-  <si>
-    <t>C107</t>
-  </si>
-  <si>
-    <t>SE limit switch status</t>
-  </si>
-  <si>
-    <t>C108</t>
-  </si>
-  <si>
-    <t>SW limit switch status</t>
-  </si>
-  <si>
-    <t>C110</t>
-  </si>
-  <si>
-    <t>Overcurrent</t>
-  </si>
-  <si>
-    <t>D120</t>
-  </si>
-  <si>
-    <t>Open timeout</t>
-  </si>
-  <si>
-    <t>D121</t>
-  </si>
-  <si>
-    <t>Close timeout</t>
-  </si>
-  <si>
-    <t>C122</t>
-  </si>
-  <si>
-    <t>Open small move timeout</t>
-  </si>
-  <si>
-    <t>C123</t>
-  </si>
-  <si>
-    <t>Close small move timeout</t>
-  </si>
-  <si>
-    <t>D130</t>
-  </si>
-  <si>
-    <t>Drive current</t>
-  </si>
-  <si>
-    <t>T0</t>
-  </si>
-  <si>
-    <t>Timout_error</t>
-  </si>
-  <si>
-    <t>dxxx</t>
-  </si>
-  <si>
-    <t>dome Counter</t>
-  </si>
-  <si>
-    <t>domve velocity</t>
-  </si>
-  <si>
-    <t>Emergency stop</t>
-  </si>
-  <si>
-    <t>C200</t>
-  </si>
-  <si>
-    <t>E-Stop</t>
-  </si>
-  <si>
-    <t>C201</t>
-  </si>
-  <si>
-    <t>E-Stop status</t>
-  </si>
-  <si>
-    <t>C202</t>
-  </si>
-  <si>
-    <t>E-relay reset.</t>
-  </si>
-  <si>
-    <t>HVAC</t>
-  </si>
-  <si>
-    <t>D500</t>
-  </si>
-  <si>
-    <t>D101</t>
-  </si>
-  <si>
-    <t>X0</t>
-  </si>
-  <si>
-    <t>Safety key</t>
-  </si>
-  <si>
-    <t>Engaged?</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>Open/Close</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>Door Power</t>
-  </si>
-  <si>
-    <t>X3</t>
-  </si>
-  <si>
-    <t>Shows actual driving state</t>
-  </si>
-  <si>
-    <t>X10</t>
-  </si>
-  <si>
-    <t>Control room lights curr det</t>
-  </si>
-  <si>
-    <t>X11</t>
-  </si>
-  <si>
-    <t>Utilities room lights curr det</t>
-  </si>
-  <si>
-    <t>X12</t>
-  </si>
-  <si>
-    <t>Spectrograph room lights curr det</t>
-  </si>
-  <si>
-    <t>X13</t>
-  </si>
-  <si>
-    <t>UMA lights curr det</t>
-  </si>
-  <si>
-    <t>X14</t>
-  </si>
-  <si>
-    <t>Tel Plat bright lights curr det</t>
-  </si>
-  <si>
-    <t>X15</t>
-  </si>
-  <si>
-    <t>Tel plat red curr det</t>
-  </si>
-  <si>
-    <t>X9</t>
-  </si>
-  <si>
-    <t>NE limit switch</t>
-  </si>
-  <si>
-    <t>NW limit switch</t>
-  </si>
-  <si>
-    <t>SE limit switch</t>
-  </si>
-  <si>
-    <t>SW limit switch</t>
-  </si>
-  <si>
-    <t>WX0</t>
-  </si>
-  <si>
-    <t>Motor counter</t>
-  </si>
-  <si>
-    <t>Y0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicator light </t>
-  </si>
-  <si>
-    <t>Bit</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>Door magnet</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
     <t>Y3</t>
   </si>
   <si>
     <t>Control room lights relay</t>
   </si>
   <si>
-    <t>Y4</t>
-  </si>
-  <si>
     <t>Utilities room lights relay</t>
   </si>
   <si>
@@ -444,28 +450,34 @@
     <t>Read/Write</t>
   </si>
   <si>
-    <t>MC0</t>
+    <t>MC1</t>
   </si>
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>MC1</t>
-  </si>
-  <si>
     <t>MC2</t>
   </si>
   <si>
     <t>MC3</t>
   </si>
   <si>
+    <t>Show actual status</t>
+  </si>
+  <si>
     <t>MC4</t>
   </si>
   <si>
+    <t>E-stop status</t>
+  </si>
+  <si>
+    <t>MC5</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
     <t>MC235</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
   <si>
     <t>MC236</t>
@@ -867,19 +879,19 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="B3" s="4" t="s">
-        <v>7</v>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>13</v>
@@ -907,130 +919,137 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E20" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -1038,86 +1057,86 @@
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1"/>
@@ -1127,105 +1146,105 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="B40" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="B41" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="B42" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="C49" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="B54" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1"/>
@@ -2232,40 +2251,40 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="4" t="s">
-        <v>99</v>
+      <c r="B5" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
@@ -2273,60 +2292,60 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1">
       <c r="F9" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -2335,45 +2354,45 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="B25" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -3402,32 +3421,32 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="4" t="s">
-        <v>125</v>
+      <c r="B4" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
@@ -3439,53 +3458,53 @@
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -3494,13 +3513,13 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -4518,7 +4537,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -4535,16 +4554,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>9</v>
@@ -4552,147 +4571,148 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>17</v>
+        <v>144</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="B7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -4701,86 +4721,86 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1"/>
@@ -4790,105 +4810,105 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1">
       <c r="B40" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1">
       <c r="B42" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="C44" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Fixed plc drive simulator issues & add drive counter variable MHR150 to modbus
</commit_message>
<xml_diff>
--- a/Documentation/PLC variables.xlsx
+++ b/Documentation/PLC variables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="178">
   <si>
     <t>Device</t>
   </si>
@@ -78,7 +78,10 @@
     <t>C4</t>
   </si>
   <si>
-    <t>E-stop ind</t>
+    <t>E- relay status</t>
+  </si>
+  <si>
+    <t>Show e-relay status</t>
   </si>
   <si>
     <t>C5</t>
@@ -246,12 +249,6 @@
     <t>Open small move timeout</t>
   </si>
   <si>
-    <t>C123</t>
-  </si>
-  <si>
-    <t>Close small move timeout</t>
-  </si>
-  <si>
     <t>D130</t>
   </si>
   <si>
@@ -264,280 +261,283 @@
     <t>Timout_error</t>
   </si>
   <si>
-    <t>dxxx</t>
+    <t>D150</t>
   </si>
   <si>
     <t>dome Counter</t>
   </si>
   <si>
+    <t>Emergency stop</t>
+  </si>
+  <si>
+    <t>C200</t>
+  </si>
+  <si>
+    <t>E-Stop</t>
+  </si>
+  <si>
+    <t>C201</t>
+  </si>
+  <si>
+    <t>E-Stop status</t>
+  </si>
+  <si>
+    <t>C202</t>
+  </si>
+  <si>
+    <t>E-relay reset.</t>
+  </si>
+  <si>
+    <t>HVAC</t>
+  </si>
+  <si>
+    <t>D500</t>
+  </si>
+  <si>
+    <t>D101</t>
+  </si>
+  <si>
+    <t>X0</t>
+  </si>
+  <si>
+    <t>Safety key</t>
+  </si>
+  <si>
+    <t>Engaged?</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Open/Close</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Door Power</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>Shows actual driving state</t>
+  </si>
+  <si>
+    <t>X10</t>
+  </si>
+  <si>
+    <t>Control room lights curr det</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>Utilities room lights curr det</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>Spectrograph room lights curr det</t>
+  </si>
+  <si>
+    <t>X13</t>
+  </si>
+  <si>
+    <t>UMA lights curr det</t>
+  </si>
+  <si>
+    <t>X14</t>
+  </si>
+  <si>
+    <t>Tel Plat bright lights curr det</t>
+  </si>
+  <si>
+    <t>X15</t>
+  </si>
+  <si>
+    <t>Tel plat red curr det</t>
+  </si>
+  <si>
+    <t>X9</t>
+  </si>
+  <si>
+    <t>NE limit switch</t>
+  </si>
+  <si>
+    <t>NW limit switch</t>
+  </si>
+  <si>
+    <t>SE limit switch</t>
+  </si>
+  <si>
+    <t>SW limit switch</t>
+  </si>
+  <si>
+    <t>WX0</t>
+  </si>
+  <si>
+    <t>Motor counter</t>
+  </si>
+  <si>
+    <t>Y0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator light </t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Door magnet</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>E-stop</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>Control room lights relay</t>
+  </si>
+  <si>
+    <t>Utilities room lights relay</t>
+  </si>
+  <si>
+    <t>Y5</t>
+  </si>
+  <si>
+    <t>Spectrograph room lights relay</t>
+  </si>
+  <si>
+    <t>Y6</t>
+  </si>
+  <si>
+    <t>UMA lights relay</t>
+  </si>
+  <si>
+    <t>Y7</t>
+  </si>
+  <si>
+    <t>Tel Plat bright lights relay</t>
+  </si>
+  <si>
+    <t>Y8</t>
+  </si>
+  <si>
+    <t>Tel plat red relay</t>
+  </si>
+  <si>
+    <t>Y9</t>
+  </si>
+  <si>
+    <t>Brake</t>
+  </si>
+  <si>
+    <t>Read/Write</t>
+  </si>
+  <si>
+    <t>MC1</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>MC2</t>
+  </si>
+  <si>
+    <t>MC3</t>
+  </si>
+  <si>
+    <t>Show actual status</t>
+  </si>
+  <si>
+    <t>MC4</t>
+  </si>
+  <si>
+    <t>E-stop status</t>
+  </si>
+  <si>
+    <t>MC5</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>MC235</t>
+  </si>
+  <si>
+    <t>MC236</t>
+  </si>
+  <si>
+    <t>MC237</t>
+  </si>
+  <si>
+    <t>MC238</t>
+  </si>
+  <si>
+    <t>MC239</t>
+  </si>
+  <si>
+    <t>MC240</t>
+  </si>
+  <si>
+    <t>MC100</t>
+  </si>
+  <si>
+    <t>MC101</t>
+  </si>
+  <si>
+    <t>MC102</t>
+  </si>
+  <si>
+    <t>MC103</t>
+  </si>
+  <si>
+    <t>MHR104-105</t>
+  </si>
+  <si>
+    <t>MC105</t>
+  </si>
+  <si>
+    <t>MC106</t>
+  </si>
+  <si>
+    <t>MC107</t>
+  </si>
+  <si>
+    <t>MC108</t>
+  </si>
+  <si>
+    <t>MC110</t>
+  </si>
+  <si>
+    <t>MHR120</t>
+  </si>
+  <si>
+    <t>MHR121</t>
+  </si>
+  <si>
+    <t>MC122</t>
+  </si>
+  <si>
+    <t>MHR130</t>
+  </si>
+  <si>
+    <t>MHR150</t>
+  </si>
+  <si>
+    <t>Dome Counter</t>
+  </si>
+  <si>
     <t>domve velocity</t>
-  </si>
-  <si>
-    <t>Emergency stop</t>
-  </si>
-  <si>
-    <t>C200</t>
-  </si>
-  <si>
-    <t>E-Stop</t>
-  </si>
-  <si>
-    <t>C201</t>
-  </si>
-  <si>
-    <t>E-Stop status</t>
-  </si>
-  <si>
-    <t>C202</t>
-  </si>
-  <si>
-    <t>E-relay reset.</t>
-  </si>
-  <si>
-    <t>HVAC</t>
-  </si>
-  <si>
-    <t>D500</t>
-  </si>
-  <si>
-    <t>D101</t>
-  </si>
-  <si>
-    <t>X0</t>
-  </si>
-  <si>
-    <t>Safety key</t>
-  </si>
-  <si>
-    <t>Engaged?</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>Open/Close</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>Door Power</t>
-  </si>
-  <si>
-    <t>X4</t>
-  </si>
-  <si>
-    <t>Shows actual driving state</t>
-  </si>
-  <si>
-    <t>X10</t>
-  </si>
-  <si>
-    <t>Control room lights curr det</t>
-  </si>
-  <si>
-    <t>X11</t>
-  </si>
-  <si>
-    <t>Utilities room lights curr det</t>
-  </si>
-  <si>
-    <t>X12</t>
-  </si>
-  <si>
-    <t>Spectrograph room lights curr det</t>
-  </si>
-  <si>
-    <t>X13</t>
-  </si>
-  <si>
-    <t>UMA lights curr det</t>
-  </si>
-  <si>
-    <t>X14</t>
-  </si>
-  <si>
-    <t>Tel Plat bright lights curr det</t>
-  </si>
-  <si>
-    <t>X15</t>
-  </si>
-  <si>
-    <t>Tel plat red curr det</t>
-  </si>
-  <si>
-    <t>X9</t>
-  </si>
-  <si>
-    <t>NE limit switch</t>
-  </si>
-  <si>
-    <t>NW limit switch</t>
-  </si>
-  <si>
-    <t>SE limit switch</t>
-  </si>
-  <si>
-    <t>SW limit switch</t>
-  </si>
-  <si>
-    <t>WX0</t>
-  </si>
-  <si>
-    <t>Motor counter</t>
-  </si>
-  <si>
-    <t>Y0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicator light </t>
-  </si>
-  <si>
-    <t>Bit</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>Door magnet</t>
-  </si>
-  <si>
-    <t>Y4</t>
-  </si>
-  <si>
-    <t>E-stop</t>
-  </si>
-  <si>
-    <t>Y3</t>
-  </si>
-  <si>
-    <t>Control room lights relay</t>
-  </si>
-  <si>
-    <t>Utilities room lights relay</t>
-  </si>
-  <si>
-    <t>Y5</t>
-  </si>
-  <si>
-    <t>Spectrograph room lights relay</t>
-  </si>
-  <si>
-    <t>Y6</t>
-  </si>
-  <si>
-    <t>UMA lights relay</t>
-  </si>
-  <si>
-    <t>Y7</t>
-  </si>
-  <si>
-    <t>Tel Plat bright lights relay</t>
-  </si>
-  <si>
-    <t>Y8</t>
-  </si>
-  <si>
-    <t>Tel plat red relay</t>
-  </si>
-  <si>
-    <t>Y9</t>
-  </si>
-  <si>
-    <t>Brake</t>
-  </si>
-  <si>
-    <t>Read/Write</t>
-  </si>
-  <si>
-    <t>MC1</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>MC2</t>
-  </si>
-  <si>
-    <t>MC3</t>
-  </si>
-  <si>
-    <t>Show actual status</t>
-  </si>
-  <si>
-    <t>MC4</t>
-  </si>
-  <si>
-    <t>E-stop status</t>
-  </si>
-  <si>
-    <t>MC5</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>MC235</t>
-  </si>
-  <si>
-    <t>MC236</t>
-  </si>
-  <si>
-    <t>MC237</t>
-  </si>
-  <si>
-    <t>MC238</t>
-  </si>
-  <si>
-    <t>MC239</t>
-  </si>
-  <si>
-    <t>MC240</t>
-  </si>
-  <si>
-    <t>MC100</t>
-  </si>
-  <si>
-    <t>MC101</t>
-  </si>
-  <si>
-    <t>MC102</t>
-  </si>
-  <si>
-    <t>MC103</t>
-  </si>
-  <si>
-    <t>MHR104-105</t>
-  </si>
-  <si>
-    <t>MC105</t>
-  </si>
-  <si>
-    <t>MC106</t>
-  </si>
-  <si>
-    <t>MC107</t>
-  </si>
-  <si>
-    <t>MC108</t>
-  </si>
-  <si>
-    <t>MC110</t>
-  </si>
-  <si>
-    <t>MHR120</t>
-  </si>
-  <si>
-    <t>MHR121</t>
-  </si>
-  <si>
-    <t>MC122</t>
-  </si>
-  <si>
-    <t>MC123</t>
-  </si>
-  <si>
-    <t>MHR130</t>
   </si>
   <si>
     <t>MC200</t>
@@ -918,13 +918,16 @@
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -933,123 +936,123 @@
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -1057,86 +1060,86 @@
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1"/>
@@ -1146,105 +1149,99 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="B40" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="B41" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="B42" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="4" t="s">
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="B48" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="C49" s="4"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="B54" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1"/>
@@ -2251,40 +2248,40 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
@@ -2292,60 +2289,60 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1">
       <c r="F9" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -2354,45 +2351,45 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="B25" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -3421,32 +3418,32 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="B4" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
@@ -3458,53 +3455,53 @@
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -3513,13 +3510,13 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -4537,7 +4534,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -4554,16 +4551,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>9</v>
@@ -4571,13 +4568,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
@@ -4590,38 +4587,38 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -4630,89 +4627,89 @@
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -4721,86 +4718,86 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1"/>
@@ -4810,76 +4807,75 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1">
       <c r="B40" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1">
       <c r="B42" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>82</v>
+      <c r="B43" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="C44" s="4" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>173</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -4887,7 +4883,7 @@
         <v>174</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -4895,12 +4891,12 @@
         <v>175</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Fixed Modbus declaration issue for the dome variables. System is now accepting remote commands.
</commit_message>
<xml_diff>
--- a/Documentation/PLC variables.xlsx
+++ b/Documentation/PLC variables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="178">
   <si>
     <t>Device</t>
   </si>
@@ -4726,6 +4726,9 @@
       <c r="C22" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="3" t="s">
@@ -4734,6 +4737,9 @@
       <c r="C23" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="3" t="s">
@@ -4742,6 +4748,9 @@
       <c r="C24" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="B25" s="3" t="s">
@@ -4750,6 +4759,9 @@
       <c r="C25" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="3" t="s">
@@ -4758,6 +4770,9 @@
       <c r="C26" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="3" t="s">
@@ -4766,6 +4781,9 @@
       <c r="C27" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="D27" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="3" t="s">
@@ -4774,6 +4792,9 @@
       <c r="C28" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="3" t="s">
@@ -4782,6 +4803,9 @@
       <c r="C29" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="3" t="s">
@@ -4789,6 +4813,9 @@
       </c>
       <c r="C30" s="4" t="s">
         <v>67</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
@@ -4799,6 +4826,9 @@
       <c r="C32" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1">
@@ -4812,6 +4842,9 @@
       <c r="C35" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="D35" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="3" t="s">
@@ -4830,6 +4863,9 @@
       </c>
       <c r="C37" s="4" t="s">
         <v>75</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -4844,6 +4880,9 @@
       <c r="C40" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="D40" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1">
@@ -4853,6 +4892,9 @@
       <c r="C42" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="D42" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="3" t="s">
@@ -4861,11 +4903,17 @@
       <c r="C43" s="3" t="s">
         <v>171</v>
       </c>
+      <c r="D43" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="C44" s="4" t="s">
         <v>172</v>
       </c>
+      <c r="D44" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
@@ -4877,6 +4925,9 @@
       <c r="C45" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="D45" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="3" t="s">
@@ -4885,6 +4936,9 @@
       <c r="C46" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="D46" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="3" t="s">
@@ -4892,6 +4946,9 @@
       </c>
       <c r="C47" s="4" t="s">
         <v>88</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Update excel file with new GS3 monitored variables. - Monitor status 2. - Frequency set point. - Output Frequency. - Output Current.
</commit_message>
<xml_diff>
--- a/Documentation/PLC variables.xlsx
+++ b/Documentation/PLC variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\3 SDSS-V\LVM\9 LVM_Enclosure_PLC\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe Besser\Desktop\3 SDSS-V\LVM\9 LVM_Enclosure_PLC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBF5AD5-81DF-4D3B-9F16-0C2093CF67AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3FBAD5-1246-4561-B8C4-3C6B00A1F04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="228">
   <si>
     <t>Device</t>
   </si>
@@ -689,6 +689,30 @@
   </si>
   <si>
     <t>MHR412</t>
+  </si>
+  <si>
+    <t>Roll-off movement</t>
+  </si>
+  <si>
+    <t>Frequency Command F</t>
+  </si>
+  <si>
+    <t>MHR413</t>
+  </si>
+  <si>
+    <t>Output Frequency</t>
+  </si>
+  <si>
+    <t>MHR414</t>
+  </si>
+  <si>
+    <t>Output Current A</t>
+  </si>
+  <si>
+    <t>MHR415</t>
+  </si>
+  <si>
+    <t>git</t>
   </si>
 </sst>
 </file>
@@ -737,28 +761,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -983,16 +1003,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.453125" customWidth="1"/>
+    <col min="1" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,57 +1033,57 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
@@ -1075,7 +1095,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1084,133 +1104,133 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
@@ -1219,7 +1239,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
         <v>47</v>
       </c>
@@ -1228,212 +1248,212 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="5"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="5"/>
+      <c r="B29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="3" t="s">
+      <c r="A30" s="5"/>
+      <c r="B30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="3" t="s">
+      <c r="A31" s="5"/>
+      <c r="B31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="3" t="s">
+      <c r="A32" s="5"/>
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="5"/>
+      <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="3" t="s">
+      <c r="A34" s="5"/>
+      <c r="B34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="3" t="s">
+      <c r="A35" s="5"/>
+      <c r="B35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="5"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="5"/>
+      <c r="B37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
+      <c r="A38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="3" t="s">
+      <c r="A40" s="5"/>
+      <c r="B40" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="5"/>
+      <c r="B41" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
+      <c r="A42" s="5"/>
       <c r="B42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="5"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="3" t="s">
+      <c r="A45" s="5"/>
+      <c r="B45" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
+      <c r="A46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="5"/>
+      <c r="B47" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
+      <c r="A48" s="5"/>
       <c r="B48" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="C49" s="3"/>
+      <c r="A49" s="5"/>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="3" t="s">
+      <c r="A51" s="5"/>
+      <c r="B51" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="3" t="s">
+      <c r="A52" s="5"/>
+      <c r="B52" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2421,16 +2441,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="29.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="1" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2451,34 +2471,34 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2486,147 +2506,147 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="F9" s="3" t="s">
+      <c r="A9" s="5"/>
+      <c r="F9" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="5"/>
+      <c r="B26" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3623,16 +3643,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="1" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3653,137 +3673,137 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4781,20 +4801,20 @@
   </sheetPr>
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" customWidth="1"/>
-    <col min="3" max="3" width="27.08984375" customWidth="1"/>
-    <col min="4" max="5" width="22.7265625" customWidth="1"/>
-    <col min="6" max="7" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="5" width="22.77734375" customWidth="1"/>
+    <col min="6" max="7" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4804,7 +4824,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -4818,13 +4838,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4833,180 +4853,180 @@
       <c r="E2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>216</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
       <c r="G5" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>49</v>
+      <c r="A22" s="6" t="s">
+        <v>220</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -5014,11 +5034,11 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -5026,11 +5046,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="5"/>
       <c r="B24" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -5038,11 +5058,11 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="5"/>
       <c r="B25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -5050,11 +5070,11 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="5"/>
       <c r="B26" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -5062,11 +5082,11 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="5"/>
       <c r="B27" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -5074,11 +5094,11 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -5086,11 +5106,11 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -5098,11 +5118,11 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="5"/>
       <c r="B30" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -5110,14 +5130,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -5125,19 +5145,19 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="5"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="5"/>
       <c r="B35" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -5145,11 +5165,11 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="5"/>
       <c r="B36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -5157,11 +5177,11 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -5169,19 +5189,19 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
+      <c r="A38" s="5"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+      <c r="A39" s="5"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+      <c r="A40" s="5"/>
       <c r="B40" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -5189,14 +5209,14 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
+      <c r="A41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="3" t="s">
+      <c r="A42" s="5"/>
+      <c r="B42" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -5204,7 +5224,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="5"/>
       <c r="B43" s="2" t="s">
         <v>167</v>
       </c>
@@ -5216,8 +5236,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="C44" s="3" t="s">
+      <c r="A44" s="5"/>
+      <c r="C44" s="2" t="s">
         <v>169</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -5225,13 +5245,13 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -5239,11 +5259,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
+      <c r="A46" s="8"/>
       <c r="B46" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -5251,11 +5271,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
+      <c r="A47" s="8"/>
       <c r="B47" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -5277,7 +5297,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="8" t="s">
         <v>215</v>
       </c>
       <c r="B51" t="s">
@@ -5291,7 +5311,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
+      <c r="A52" s="8"/>
       <c r="B52" t="s">
         <v>192</v>
       </c>
@@ -5303,7 +5323,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
+      <c r="A53" s="8"/>
       <c r="B53" t="s">
         <v>193</v>
       </c>
@@ -5315,7 +5335,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
+      <c r="A54" s="8"/>
       <c r="B54" t="s">
         <v>194</v>
       </c>
@@ -5327,7 +5347,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
+      <c r="A55" s="8"/>
       <c r="B55" t="s">
         <v>195</v>
       </c>
@@ -5339,7 +5359,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
+      <c r="A56" s="8"/>
       <c r="B56" t="s">
         <v>196</v>
       </c>
@@ -5351,7 +5371,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
+      <c r="A57" s="8"/>
       <c r="B57" t="s">
         <v>209</v>
       </c>
@@ -5363,7 +5383,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
+      <c r="A58" s="8"/>
       <c r="B58" t="s">
         <v>210</v>
       </c>
@@ -5375,7 +5395,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
+      <c r="A59" s="8"/>
       <c r="B59" t="s">
         <v>211</v>
       </c>
@@ -5387,7 +5407,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
+      <c r="A60" s="8"/>
       <c r="B60" t="s">
         <v>212</v>
       </c>
@@ -5399,7 +5419,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
+      <c r="A61" s="8"/>
       <c r="B61" t="s">
         <v>213</v>
       </c>
@@ -5411,7 +5431,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
+      <c r="A62" s="8"/>
       <c r="B62" t="s">
         <v>214</v>
       </c>
@@ -6375,16 +6395,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBE9CBA-0D72-45D2-BCD9-E22B13DC8DB6}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="A10:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6583,6 +6603,44 @@
         <v>219</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15">
+        <v>48451</v>
+      </c>
+      <c r="D15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16">
+        <v>48452</v>
+      </c>
+      <c r="D16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C17">
+        <v>48453</v>
+      </c>
+      <c r="D17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Motor encoder added as input
Motor encoder enabled as input

MHR150 has the encoders raw count.
MHR151 has the theoretical distance moved by the chain in mm.
MHR152 has the measured gap off the roof in mm.
</commit_message>
<xml_diff>
--- a/Documentation/PLC variables.xlsx
+++ b/Documentation/PLC variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe Besser\Desktop\3 SDSS-V\LVM\9 LVM_Enclosure_PLC\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nas02.lco.cl\USERS_HOMES\Felipe Besser\3 SDSS-V\LVM\9 LVM_Enclosure_PLC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E1B01D-33BA-4DC4-A8BE-D852B00B74E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5A30E0-751B-4926-AB0B-8C64303625B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="248">
   <si>
     <t>Device</t>
   </si>
@@ -376,9 +376,6 @@
     <t>Dome Counter</t>
   </si>
   <si>
-    <t>domve velocity</t>
-  </si>
-  <si>
     <t>MC200</t>
   </si>
   <si>
@@ -388,12 +385,6 @@
     <t>MC202</t>
   </si>
   <si>
-    <t>MHR500</t>
-  </si>
-  <si>
-    <t>MHR501</t>
-  </si>
-  <si>
     <t>GS3 code</t>
   </si>
   <si>
@@ -568,21 +559,9 @@
     <t>Motor current RPM</t>
   </si>
   <si>
-    <t>Sensor 1 (Utilities room) reading</t>
-  </si>
-  <si>
-    <t>Sensor 2 (Spectrograph room) reading</t>
-  </si>
-  <si>
     <t>MHR603</t>
   </si>
   <si>
-    <t>Sensor 1 (Utilities room) mode</t>
-  </si>
-  <si>
-    <t>Sensor 2 (Spectrograph room) mode</t>
-  </si>
-  <si>
     <t>Control room lights toggle</t>
   </si>
   <si>
@@ -628,12 +607,6 @@
     <t>MHR605</t>
   </si>
   <si>
-    <t>Sensor 1 (Utilities room) Error</t>
-  </si>
-  <si>
-    <t>Sensor 2 (Spectrograph room) Error</t>
-  </si>
-  <si>
     <t>DeviMCe</t>
   </si>
   <si>
@@ -664,18 +637,6 @@
     <t>Drive Current</t>
   </si>
   <si>
-    <t>MC1000</t>
-  </si>
-  <si>
-    <t>MC1001</t>
-  </si>
-  <si>
-    <t>MC1002</t>
-  </si>
-  <si>
-    <t>MC1003</t>
-  </si>
-  <si>
     <t>Hearthbeat</t>
   </si>
   <si>
@@ -691,15 +652,9 @@
     <t>Drive velocity</t>
   </si>
   <si>
-    <t>MC1006</t>
-  </si>
-  <si>
     <t>Dome closed</t>
   </si>
   <si>
-    <t>MC1007</t>
-  </si>
-  <si>
     <t>X39</t>
   </si>
   <si>
@@ -758,6 +713,66 @@
   </si>
   <si>
     <t>Local enable</t>
+  </si>
+  <si>
+    <t>dome velocity</t>
+  </si>
+  <si>
+    <t>ODH Sensor</t>
+  </si>
+  <si>
+    <t>MHR600</t>
+  </si>
+  <si>
+    <t>MHR601</t>
+  </si>
+  <si>
+    <t>MHR602</t>
+  </si>
+  <si>
+    <t>Heartbeat input</t>
+  </si>
+  <si>
+    <t>Heartbeat aknowledge</t>
+  </si>
+  <si>
+    <t>Heartbeat error</t>
+  </si>
+  <si>
+    <t>MC109</t>
+  </si>
+  <si>
+    <t>Rain sensor</t>
+  </si>
+  <si>
+    <t>X47</t>
+  </si>
+  <si>
+    <t>Rain sensor NC output</t>
+  </si>
+  <si>
+    <t>Environmental</t>
+  </si>
+  <si>
+    <t>MC700</t>
+  </si>
+  <si>
+    <t>Rain sensor output</t>
+  </si>
+  <si>
+    <t>MHR700</t>
+  </si>
+  <si>
+    <t>Rain conunter (will count every time the rain sensor transitions from 1 to 0</t>
+  </si>
+  <si>
+    <t>MHR151</t>
+  </si>
+  <si>
+    <t>Dome pos in mm (theoretical)</t>
+  </si>
+  <si>
+    <t>Dome pos in mm (scale function)</t>
   </si>
 </sst>
 </file>
@@ -780,10 +795,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -837,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -850,6 +867,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -864,8 +884,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1102,13 +1122,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1117,11 +1137,11 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1135,7 +1155,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>96</v>
       </c>
@@ -1147,7 +1167,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>96</v>
       </c>
@@ -1159,7 +1179,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>97</v>
       </c>
@@ -1171,9 +1191,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1183,28 +1203,28 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1218,7 +1238,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
         <v>100</v>
       </c>
@@ -1230,7 +1250,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>101</v>
       </c>
@@ -1242,7 +1262,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>102</v>
       </c>
@@ -1254,7 +1274,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>103</v>
       </c>
@@ -1266,7 +1286,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>104</v>
       </c>
@@ -1278,9 +1298,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>26</v>
@@ -1288,9 +1308,9 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>27</v>
@@ -1298,9 +1318,9 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>28</v>
@@ -1308,9 +1328,9 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>29</v>
@@ -1318,34 +1338,34 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1356,7 +1376,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
         <v>106</v>
       </c>
@@ -1365,7 +1385,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
         <v>107</v>
       </c>
@@ -1374,7 +1394,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="2" t="s">
         <v>108</v>
       </c>
@@ -1383,16 +1403,16 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
         <v>109</v>
       </c>
@@ -1401,7 +1421,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="2" t="s">
         <v>110</v>
       </c>
@@ -1410,7 +1430,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="2" t="s">
         <v>111</v>
       </c>
@@ -1419,7 +1439,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="2" t="s">
         <v>112</v>
       </c>
@@ -1428,27 +1448,27 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
+      <c r="A36" s="10"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1477,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="2" t="s">
         <v>44</v>
       </c>
@@ -1466,36 +1486,36 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="9"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="2" t="s">
         <v>48</v>
       </c>
@@ -1504,7 +1524,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="9"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="2" t="s">
         <v>50</v>
       </c>
@@ -1513,33 +1533,33 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="9"/>
+      <c r="A49" s="10"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>208</v>
+      <c r="A50" s="12" t="s">
+        <v>199</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="9"/>
+      <c r="A51" s="10"/>
       <c r="B51" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="9"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>55</v>
@@ -2521,8 +2541,8 @@
   </sheetPr>
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2555,64 +2575,64 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="F8" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2623,7 +2643,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
         <v>62</v>
       </c>
@@ -2632,7 +2652,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
         <v>64</v>
       </c>
@@ -2641,7 +2661,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>66</v>
       </c>
@@ -2650,75 +2670,75 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="5" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>74</v>
       </c>
@@ -2726,7 +2746,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3717,7 +3747,7 @@
   </sheetPr>
   <dimension ref="A1:F988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -3751,29 +3781,29 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>79</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3784,7 +3814,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="5" t="s">
         <v>77</v>
       </c>
@@ -3793,16 +3823,16 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>80</v>
       </c>
@@ -3811,7 +3841,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="5" t="s">
         <v>78</v>
       </c>
@@ -3820,7 +3850,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="5" t="s">
         <v>83</v>
       </c>
@@ -3847,10 +3877,10 @@
         <v>89</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4847,10 +4877,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1006"/>
+  <dimension ref="A1:G1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4886,14 +4916,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>241</v>
+      <c r="C2" s="8" t="s">
+        <v>226</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>95</v>
@@ -4909,7 +4939,7 @@
         <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>95</v>
@@ -4922,7 +4952,7 @@
         <v>97</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>95</v>
@@ -4930,790 +4960,819 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E18" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="2" t="s">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2" t="s">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2" t="s">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="2" t="s">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D23" s="2" t="s">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="10"/>
+      <c r="B30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="C31" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="5" t="s">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" t="s">
-        <v>133</v>
-      </c>
-      <c r="D29" t="s">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10"/>
+      <c r="B34" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="B30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" t="s">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="B31" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" t="s">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="B32" t="s">
-        <v>140</v>
-      </c>
-      <c r="C32" t="s">
-        <v>132</v>
-      </c>
-      <c r="D32" t="s">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C33" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="B34" t="s">
-        <v>142</v>
-      </c>
-      <c r="C34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" t="s">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D35" s="4" t="s">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10"/>
+      <c r="B40" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="4" t="s">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="B38" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>38</v>
+        <v>245</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>39</v>
+        <v>113</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="2" t="s">
-        <v>213</v>
-      </c>
+      <c r="A44" s="10"/>
       <c r="C44" s="2" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
+      <c r="A45" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="B45" s="2" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
+      <c r="A46" s="14"/>
       <c r="B46" s="2" t="s">
-        <v>220</v>
+        <v>116</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>221</v>
+        <v>53</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" t="s">
+        <v>130</v>
+      </c>
+      <c r="D48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="9"/>
-      <c r="B47" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D47" s="2" t="s">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="9"/>
-      <c r="B48" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" s="2" t="s">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="9"/>
-      <c r="C49" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="2" t="s">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="2" t="s">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
-      <c r="B51" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13"/>
-      <c r="B52" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>119</v>
+      <c r="A53" s="14"/>
+      <c r="B53" t="s">
+        <v>139</v>
+      </c>
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
-        <v>156</v>
-      </c>
+      <c r="A54" s="14"/>
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D56" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="13"/>
+      <c r="A57" s="14"/>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D57" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="13"/>
+      <c r="A58" s="14"/>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D58" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="13"/>
+      <c r="A59" s="14"/>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D59" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13"/>
+      <c r="A60" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="B60" t="s">
-        <v>141</v>
-      </c>
-      <c r="C60" t="s">
-        <v>135</v>
-      </c>
-      <c r="D60" t="s">
-        <v>95</v>
+        <v>203</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="13"/>
+      <c r="A61" s="14"/>
       <c r="B61" t="s">
-        <v>142</v>
-      </c>
-      <c r="C61" t="s">
-        <v>136</v>
+        <v>204</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="D61" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
+      <c r="A62" s="14"/>
       <c r="B62" t="s">
-        <v>150</v>
-      </c>
-      <c r="C62" t="s">
-        <v>144</v>
+        <v>205</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="D62" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="13"/>
-      <c r="B63" t="s">
-        <v>151</v>
-      </c>
-      <c r="C63" t="s">
-        <v>145</v>
+      <c r="A63" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="D63" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="13"/>
-      <c r="B64" t="s">
-        <v>152</v>
-      </c>
-      <c r="C64" t="s">
-        <v>146</v>
+      <c r="A64" s="15"/>
+      <c r="B64" s="7" t="s">
+        <v>231</v>
       </c>
       <c r="D64" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="13"/>
-      <c r="B65" t="s">
-        <v>153</v>
-      </c>
-      <c r="C65" t="s">
-        <v>147</v>
+      <c r="A65" s="15"/>
+      <c r="B65" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="D65" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="13"/>
-      <c r="B66" t="s">
-        <v>154</v>
-      </c>
-      <c r="C66" t="s">
-        <v>148</v>
+      <c r="A66" s="15"/>
+      <c r="B66" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="D66" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="13"/>
-      <c r="B67" t="s">
-        <v>155</v>
-      </c>
-      <c r="C67" t="s">
-        <v>149</v>
+      <c r="A67" s="15"/>
+      <c r="B67" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="D67" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="B68" t="s">
-        <v>216</v>
-      </c>
-      <c r="C68" t="s">
-        <v>179</v>
+      <c r="A68" s="15"/>
+      <c r="B68" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="D68" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
-      <c r="B69" t="s">
-        <v>217</v>
+      <c r="A69" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="C69" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="D69" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="13"/>
-      <c r="B70" t="s">
-        <v>218</v>
+      <c r="A70" s="14"/>
+      <c r="B70" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="C70" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="D70" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="13"/>
-      <c r="B71" t="s">
-        <v>181</v>
-      </c>
-      <c r="C71" t="s">
-        <v>183</v>
-      </c>
-      <c r="D71" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="13"/>
-      <c r="B72" t="s">
-        <v>197</v>
-      </c>
-      <c r="C72" t="s">
-        <v>199</v>
-      </c>
-      <c r="D72" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="13"/>
-      <c r="B73" t="s">
-        <v>198</v>
-      </c>
-      <c r="C73" t="s">
-        <v>200</v>
-      </c>
-      <c r="D73" t="s">
-        <v>95</v>
-      </c>
-    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6647,14 +6706,18 @@
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A12:A23"/>
-    <mergeCell ref="A24:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A56:A67"/>
+  <mergeCells count="8">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A48:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A5:A16"/>
+    <mergeCell ref="A17:A44"/>
+    <mergeCell ref="A45:A47"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6678,174 +6741,174 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C2">
         <v>41568</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C3">
         <v>41569</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C4">
         <v>41570</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C5">
         <v>41571</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>41572</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C7">
         <v>41573</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C8">
         <v>42331</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C9">
         <v>48449</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C10">
         <v>48450</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C11">
         <v>48451</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C12">
         <v>48452</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C13">
         <v>48453</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documentation for V0.93
</commit_message>
<xml_diff>
--- a/Documentation/PLC variables.xlsx
+++ b/Documentation/PLC variables.xlsx
@@ -8,20 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nas02.lco.cl\USERS_HOMES\Felipe Besser\3 SDSS-V\LVM\9 LVM_Enclosure_PLC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233E21B9-A7FC-45F0-8749-9AB2BCA007CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A56BC5C-789D-4941-B2EA-4DD0A2D3A97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Variables" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Input" sheetId="2" r:id="rId2"/>
     <sheet name="Output" sheetId="3" r:id="rId3"/>
     <sheet name="Modbus" sheetId="4" r:id="rId4"/>
     <sheet name="GS3 read" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Modbus!$A$1:$G$999</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="252">
   <si>
     <t>Device</t>
   </si>
@@ -55,12 +52,63 @@
     <t>Interlock</t>
   </si>
   <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>show key position</t>
+  </si>
+  <si>
+    <t>Door status</t>
+  </si>
+  <si>
+    <t>Door open/close</t>
+  </si>
+  <si>
+    <t>Door power</t>
+  </si>
+  <si>
+    <t>Magnet lock powered on/off</t>
+  </si>
+  <si>
+    <t>drive interlock state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show actual </t>
+  </si>
+  <si>
+    <t>E- relay status</t>
+  </si>
+  <si>
+    <t>Show e-relay status</t>
+  </si>
+  <si>
+    <t>E-stop modbus</t>
+  </si>
+  <si>
     <t>Lights</t>
   </si>
   <si>
+    <t>Control room lights new status</t>
+  </si>
+  <si>
     <t>Changes relay</t>
   </si>
   <si>
+    <t>Utilities room lights new status</t>
+  </si>
+  <si>
+    <t>Spectrograph room lights new status</t>
+  </si>
+  <si>
+    <t>UMA lights new status</t>
+  </si>
+  <si>
+    <t>Tel Plat bright lights new status</t>
+  </si>
+  <si>
+    <t>Tel plat red new status</t>
+  </si>
+  <si>
     <t>Control room lights status</t>
   </si>
   <si>
@@ -76,15 +124,27 @@
     <t>Tel Plat bright lights status</t>
   </si>
   <si>
+    <t>Tel plat red status</t>
+  </si>
+  <si>
     <t>Shutter movement</t>
   </si>
   <si>
     <t>Drive enable</t>
   </si>
   <si>
+    <t>Drive state</t>
+  </si>
+  <si>
     <t>Motor direction</t>
   </si>
   <si>
+    <t>Drive brake</t>
+  </si>
+  <si>
+    <t>D104-105</t>
+  </si>
+  <si>
     <t>NE limit switch status</t>
   </si>
   <si>
@@ -97,6 +157,36 @@
     <t>SW limit switch status</t>
   </si>
   <si>
+    <t>D120</t>
+  </si>
+  <si>
+    <t>Open timeout</t>
+  </si>
+  <si>
+    <t>D121</t>
+  </si>
+  <si>
+    <t>Close timeout</t>
+  </si>
+  <si>
+    <t>Open small move timeout</t>
+  </si>
+  <si>
+    <t>D130</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>Timout_error</t>
+  </si>
+  <si>
+    <t>D150</t>
+  </si>
+  <si>
+    <t>dome Counter</t>
+  </si>
+  <si>
     <t>Emergency stop</t>
   </si>
   <si>
@@ -121,15 +211,30 @@
     <t>Shows actual driving state</t>
   </si>
   <si>
+    <t>X10</t>
+  </si>
+  <si>
     <t>Control room lights curr det</t>
   </si>
   <si>
+    <t>X11</t>
+  </si>
+  <si>
     <t>Utilities room lights curr det</t>
   </si>
   <si>
+    <t>X12</t>
+  </si>
+  <si>
     <t>Spectrograph room lights curr det</t>
   </si>
   <si>
+    <t>X13</t>
+  </si>
+  <si>
+    <t>UMA lights curr det</t>
+  </si>
+  <si>
     <t>Tel Plat bright lights curr det</t>
   </si>
   <si>
@@ -181,9 +286,15 @@
     <t>Spectrograph room lights relay</t>
   </si>
   <si>
+    <t>Y6</t>
+  </si>
+  <si>
     <t>UMA lights relay</t>
   </si>
   <si>
+    <t>Y7</t>
+  </si>
+  <si>
     <t>Tel Plat bright lights relay</t>
   </si>
   <si>
@@ -196,6 +307,9 @@
     <t>Y9</t>
   </si>
   <si>
+    <t>Brake</t>
+  </si>
+  <si>
     <t>Read/Write</t>
   </si>
   <si>
@@ -235,6 +349,9 @@
     <t>MC100</t>
   </si>
   <si>
+    <t>MC101</t>
+  </si>
+  <si>
     <t>MC102</t>
   </si>
   <si>
@@ -340,12 +457,42 @@
     <t>Serial Comm (RS-485) Speed Reference</t>
   </si>
   <si>
+    <t>Serial Comm RUN Command</t>
+  </si>
+  <si>
+    <t>Serial Comm Direction Command</t>
+  </si>
+  <si>
+    <t>Serial Comm External Fault</t>
+  </si>
+  <si>
+    <t>Serial Comm Fault Reset</t>
+  </si>
+  <si>
+    <t>Serial Comm JOG Command</t>
+  </si>
+  <si>
+    <t>MHR406</t>
+  </si>
+  <si>
+    <t>MHR407</t>
+  </si>
+  <si>
+    <t>MHR408</t>
+  </si>
+  <si>
+    <t>MHR409</t>
+  </si>
+  <si>
     <t>MHR410</t>
   </si>
   <si>
     <t>MHR411</t>
   </si>
   <si>
+    <t>GS3 Status</t>
+  </si>
+  <si>
     <t>Status monitor 2</t>
   </si>
   <si>
@@ -394,6 +541,9 @@
     <t>Status Monitor 1</t>
   </si>
   <si>
+    <t>Frequency Command</t>
+  </si>
+  <si>
     <t>Output Current</t>
   </si>
   <si>
@@ -466,12 +616,27 @@
     <t>DesMCription</t>
   </si>
   <si>
+    <t>MC4</t>
+  </si>
+  <si>
+    <t>MC5</t>
+  </si>
+  <si>
     <t>MC110</t>
   </si>
   <si>
+    <t>MC122</t>
+  </si>
+  <si>
     <t>EmergenMCy stop</t>
   </si>
   <si>
+    <t>OverCurrent</t>
+  </si>
+  <si>
+    <t>Drive Current</t>
+  </si>
+  <si>
     <t>Hearthbeat</t>
   </si>
   <si>
@@ -484,9 +649,15 @@
     <t>MC602</t>
   </si>
   <si>
+    <t>Drive velocity</t>
+  </si>
+  <si>
     <t>Dome closed</t>
   </si>
   <si>
+    <t>X39</t>
+  </si>
+  <si>
     <t>X38</t>
   </si>
   <si>
@@ -523,6 +694,9 @@
     <t>X29</t>
   </si>
   <si>
+    <t>X30</t>
+  </si>
+  <si>
     <t>X32</t>
   </si>
   <si>
@@ -541,6 +715,9 @@
     <t>Local enable</t>
   </si>
   <si>
+    <t>dome velocity</t>
+  </si>
+  <si>
     <t>ODH Sensor</t>
   </si>
   <si>
@@ -592,163 +769,22 @@
     <t>MHR151</t>
   </si>
   <si>
-    <t>Dome pos in mm</t>
+    <t>Dome pos in mm (theoretical)</t>
+  </si>
+  <si>
+    <t>Dome pos in mm (scale function)</t>
   </si>
   <si>
     <t>MHR152</t>
   </si>
   <si>
-    <t>MC111</t>
-  </si>
-  <si>
-    <t>Roll-off lockout</t>
-  </si>
-  <si>
-    <t>MC112</t>
-  </si>
-  <si>
-    <t>Roll-off error</t>
-  </si>
-  <si>
-    <t>Start brake</t>
-  </si>
-  <si>
-    <t>Drive speed A</t>
-  </si>
-  <si>
-    <t>Drive speed B</t>
-  </si>
-  <si>
-    <t>V100</t>
-  </si>
-  <si>
-    <t>V101</t>
-  </si>
-  <si>
-    <t>Deprecated</t>
-  </si>
-  <si>
-    <t>Dome_tout_stat</t>
-  </si>
-  <si>
-    <t>old Roll-off timeout status</t>
-  </si>
-  <si>
-    <t>MC104</t>
-  </si>
-  <si>
-    <t>Dome_Tout_rst</t>
-  </si>
-  <si>
-    <t>old Reset Roll-off timeout bit</t>
-  </si>
-  <si>
-    <t>MC113</t>
-  </si>
-  <si>
-    <t>Roll-off error reset</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>MC900</t>
-  </si>
-  <si>
-    <t>Engineering hardware mode</t>
-  </si>
-  <si>
-    <t>W/R</t>
-  </si>
-  <si>
-    <t>Disables hardware safety features</t>
-  </si>
-  <si>
-    <t>Disables software safety features</t>
-  </si>
-  <si>
-    <t>MC901</t>
-  </si>
-  <si>
-    <t>Engineering software mode</t>
-  </si>
-  <si>
-    <t>MHR130</t>
-  </si>
-  <si>
-    <t>Copied from MHR415</t>
-  </si>
-  <si>
-    <t>Dome speed in mm/s</t>
-  </si>
-  <si>
-    <t>Not yet implemented</t>
-  </si>
-  <si>
-    <t>Frequency Command (desired freq)</t>
-  </si>
-  <si>
-    <t>ODH O2 utilities room</t>
-  </si>
-  <si>
-    <t>in percent decimal</t>
-  </si>
-  <si>
-    <t>ODH O2 spectrograph room</t>
-  </si>
-  <si>
-    <t>ODH error code utilities room</t>
-  </si>
-  <si>
-    <t>ODH error code spectrograph room</t>
-  </si>
-  <si>
-    <t>ODH status byte utilities room</t>
-  </si>
-  <si>
-    <t>ODH status byte spectrograph room</t>
-  </si>
-  <si>
-    <t>MHR701</t>
-  </si>
-  <si>
-    <t>No rain countdown</t>
-  </si>
-  <si>
-    <t>15 min countdown</t>
-  </si>
-  <si>
-    <t>Enclosure</t>
-  </si>
-  <si>
-    <t>X24</t>
-  </si>
-  <si>
-    <t>X25</t>
-  </si>
-  <si>
-    <t>X26</t>
-  </si>
-  <si>
-    <t>X27</t>
-  </si>
-  <si>
-    <t>X28</t>
-  </si>
-  <si>
-    <t>Mezzanine lights curr det</t>
-  </si>
-  <si>
-    <t>X36</t>
-  </si>
-  <si>
-    <t>Motor brake</t>
-  </si>
-  <si>
-    <t>Y14</t>
-  </si>
-  <si>
-    <t>Y13</t>
+    <t>MC99</t>
+  </si>
+  <si>
+    <t>Dome mode selector</t>
+  </si>
+  <si>
+    <t>Selects between normal operation and overcurrent only mode.</t>
   </si>
 </sst>
 </file>
@@ -830,24 +866,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -865,10 +898,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1090,8 +1119,8 @@
   </sheetPr>
   <dimension ref="A1:F1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1105,13 +1134,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1120,271 +1149,433 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
+      <c r="A24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
+      <c r="A25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
+      <c r="A26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>14</v>
+      <c r="A27" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>195</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>193</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
-        <v>196</v>
+        <v>106</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>194</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
+      <c r="A36" s="10"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
+      <c r="A38" s="10"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
+      <c r="A44" s="10"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
+      <c r="A46" s="10"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11"/>
+      <c r="A49" s="10"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="11"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
@@ -2362,8 +2553,8 @@
   </sheetPr>
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2396,188 +2587,186 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>228</v>
-      </c>
+      <c r="A2" s="10"/>
       <c r="B2" s="2" t="s">
-        <v>158</v>
+        <v>216</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>167</v>
+        <v>226</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>159</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A8" s="10"/>
       <c r="F8" s="2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>7</v>
+      <c r="A11" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
-        <v>230</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
-        <v>231</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
-        <v>232</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>234</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>235</v>
+      <c r="B21" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
-        <v>163</v>
+        <v>222</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="4" t="s">
-        <v>151</v>
+      <c r="A23" s="10"/>
+      <c r="B23" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
-        <v>164</v>
+        <v>223</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>178</v>
+        <v>238</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3571,7 +3760,7 @@
   <dimension ref="A1:F988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3604,111 +3793,109 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>154</v>
+      <c r="A2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>155</v>
+      <c r="A3" s="9"/>
+      <c r="B3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>40</v>
+      <c r="A4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="4" t="s">
-        <v>41</v>
+      <c r="A5" s="9"/>
+      <c r="B5" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="4" t="s">
-        <v>153</v>
+      <c r="A6" s="9"/>
+      <c r="B6" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="4" t="s">
-        <v>44</v>
+      <c r="A7" s="9"/>
+      <c r="B7" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="4" t="s">
-        <v>42</v>
+      <c r="A8" s="9"/>
+      <c r="B8" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="4" t="s">
-        <v>47</v>
+      <c r="A9" s="9"/>
+      <c r="B9" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>236</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-    </row>
+      <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3723,7 +3910,7 @@
     <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="6"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4702,10 +4889,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G998"/>
+  <dimension ref="A1:G1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4728,7 +4915,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -4741,865 +4928,887 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>167</v>
+        <v>94</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>226</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
-        <v>134</v>
+        <v>185</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
-        <v>135</v>
+        <v>186</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>138</v>
+        <v>189</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>59</v>
+      <c r="A17" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
-      <c r="B18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>116</v>
+      <c r="B18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
-      <c r="B19" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>59</v>
+      <c r="B19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>198</v>
+        <v>165</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G20" t="s">
-        <v>199</v>
+        <v>98</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
-      <c r="B21" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G21" t="s">
-        <v>202</v>
+      <c r="B21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>56</v>
+      <c r="B22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>56</v>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
-      <c r="B24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>56</v>
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
-      <c r="B25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>56</v>
+      <c r="B25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
-      <c r="B26" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>56</v>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
-      <c r="B27" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>56</v>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
-      <c r="B28" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>56</v>
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
-      <c r="B29" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>56</v>
+      <c r="B29" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
-      <c r="B30" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>59</v>
+      <c r="B30" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
-      <c r="B31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>56</v>
+      <c r="B31" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
-      <c r="B32" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
-      <c r="B33" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
-      <c r="B34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
-      <c r="B37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C38" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" t="s">
-        <v>56</v>
-      </c>
-      <c r="F38" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="B39" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="B43" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
-      <c r="B44" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F45" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
-      <c r="B46" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="15"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14"/>
       <c r="B48" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>22</v>
+        <v>117</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" t="s">
+        <v>130</v>
+      </c>
+      <c r="D49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+      <c r="B51" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+      <c r="B54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+      <c r="B56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C56" t="s">
+        <v>142</v>
+      </c>
+      <c r="D56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+      <c r="B57" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+      <c r="B58" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" t="s">
+        <v>144</v>
+      </c>
+      <c r="D58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="14"/>
+      <c r="B59" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="14"/>
+      <c r="B60" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" t="s">
         <v>146</v>
       </c>
-      <c r="B50" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" t="s">
-        <v>148</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" t="s">
-        <v>149</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C53" t="s">
-        <v>218</v>
-      </c>
-      <c r="D53" t="s">
-        <v>56</v>
-      </c>
-      <c r="F53" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16"/>
-      <c r="B54" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C54" t="s">
-        <v>220</v>
-      </c>
-      <c r="D54" t="s">
-        <v>56</v>
-      </c>
-      <c r="F54" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="16"/>
-      <c r="B55" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C55" t="s">
-        <v>221</v>
-      </c>
-      <c r="D55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="16"/>
-      <c r="B56" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" t="s">
-        <v>222</v>
-      </c>
-      <c r="D56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="16"/>
-      <c r="B57" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C57" t="s">
-        <v>223</v>
-      </c>
-      <c r="D57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="16"/>
-      <c r="B58" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C58" t="s">
-        <v>224</v>
-      </c>
-      <c r="D58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C59" t="s">
-        <v>182</v>
-      </c>
-      <c r="D59" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
-      <c r="B60" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C60" t="s">
-        <v>184</v>
-      </c>
       <c r="D60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="15"/>
-      <c r="B61" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C61" t="s">
-        <v>226</v>
-      </c>
-      <c r="D61" t="s">
-        <v>56</v>
-      </c>
-      <c r="F61" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" t="s">
+        <v>203</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14"/>
+      <c r="B62" t="s">
+        <v>204</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="14"/>
+      <c r="B63" t="s">
         <v>205</v>
       </c>
-      <c r="B62" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C62" t="s">
-        <v>207</v>
-      </c>
-      <c r="D62" t="s">
-        <v>208</v>
-      </c>
-      <c r="F62" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
-      <c r="B63" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C63" t="s">
-        <v>212</v>
+      <c r="C63" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
-      </c>
-      <c r="F63" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="15"/>
+      <c r="B65" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="15"/>
+      <c r="B66" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="15"/>
+      <c r="B67" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="15"/>
+      <c r="B68" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D68" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="15"/>
+      <c r="B69" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C70" t="s">
+        <v>242</v>
+      </c>
+      <c r="D70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="14"/>
+      <c r="B71" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C71" t="s">
+        <v>244</v>
+      </c>
+      <c r="D71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6518,17 +6727,27 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:G1002" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <mergeCells count="8">
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A59:A61"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A49:A60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="A70:A71"/>
     <mergeCell ref="A5:A16"/>
-    <mergeCell ref="A17:A46"/>
-    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A17:A45"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6541,7 +6760,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6552,174 +6771,174 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="C2">
         <v>41568</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="C3">
         <v>41569</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="C4">
         <v>41570</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C5">
         <v>41571</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>41572</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="C7">
         <v>41573</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C8">
         <v>42331</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="C9">
         <v>48449</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
       <c r="C10">
         <v>48450</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="C11">
         <v>48451</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C12">
         <v>48452</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="C13">
         <v>48453</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>